<commit_message>
UPDATED TILL - 29-08-2020
</commit_message>
<xml_diff>
--- a/docs/Add-Service.xlsx
+++ b/docs/Add-Service.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\BGVHWD-master\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E751410-D090-4A75-9446-7BBDBB6A5568}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FADE36-1D9A-4694-91FE-FA027502EF1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D52E3EEF-53E6-4372-B35F-0894A6C3E55A}"/>
   </bookViews>
@@ -1764,7 +1764,7 @@
   <dimension ref="A1:XFB247"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3783,7 +3783,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="uDgnTJZS60Yh2OoWM1myli+ncSEz13g28/fxBl9vqZPrA694RQr48tcnwz6cdUKLzWaHPgNmHlcpuhnodeUZDA==" saltValue="07EB29YVprzim3Rvd8vF3w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="q1q/uRadfYEXi5/8SXcSRvUhGHUgzfHhF2vBgJPtqfy3CX7vTyfQbOsMocHXpR8pmt27M0MEPjJo8DAw+dRSdA==" saltValue="jSyfNN4oQg+J3Hor+HIokA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A4:D4"/>

</xml_diff>

<commit_message>
UPDATED TILL - 17-09-2020
</commit_message>
<xml_diff>
--- a/docs/Add-Service.xlsx
+++ b/docs/Add-Service.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\BGVHWD-master\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB689B5B-EBCF-464E-BD5E-9232D68E514F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03715E5C-1657-4777-A961-0E5CBF77DEE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D52E3EEF-53E6-4372-B35F-0894A6C3E55A}"/>
   </bookViews>
@@ -551,7 +551,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>